<commit_message>
Sidrac + similarity graphs
</commit_message>
<xml_diff>
--- a/data/metadata_corrected.xlsx
+++ b/data/metadata_corrected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinevandyck/Code/boendale-authorship/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinevandyck/Code/authorship-boendale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCA3CBC-5F94-9E44-8AF6-4E6854E4D1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841E83E7-D309-B341-AAC0-0771E0D86FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="612">
   <si>
     <t>id</t>
   </si>
@@ -1857,6 +1857,18 @@
   </si>
   <si>
     <t>Brabantsche yeesten (B5)</t>
+  </si>
+  <si>
+    <t>sidrac</t>
+  </si>
+  <si>
+    <t>Sidrac</t>
+  </si>
+  <si>
+    <t>1318-1329</t>
+  </si>
+  <si>
+    <t>Proza</t>
   </si>
 </sst>
 </file>
@@ -2242,10 +2254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H289"/>
+  <dimension ref="A1:H290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="144" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A272" zoomScale="144" workbookViewId="0">
+      <selection activeCell="A295" sqref="A295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8194,6 +8206,29 @@
         <v>540</v>
       </c>
     </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A290" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B290" t="s">
+        <v>609</v>
+      </c>
+      <c r="C290" t="s">
+        <v>127</v>
+      </c>
+      <c r="D290" t="s">
+        <v>9</v>
+      </c>
+      <c r="E290" t="s">
+        <v>610</v>
+      </c>
+      <c r="F290" t="s">
+        <v>611</v>
+      </c>
+      <c r="G290" t="s">
+        <v>611</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I287">
     <sortCondition ref="B225:B287"/>

</xml_diff>